<commit_message>
Add， 2022 9S feature calculate sbatch
</commit_message>
<xml_diff>
--- a/data_input/SI_for_ML.xlsx
+++ b/data_input/SI_for_ML.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qizhou/#file/2_projects/FI_paper/2tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qizhou/#python/#GitHub_saved/ML-BL-enhance-DF-EWs/data_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9D90CF-0DC5-3F47-95F3-907B6474A3F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0296087-FC24-A749-9968-9555024F06E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4220" windowWidth="28800" windowHeight="16020" activeTab="2" xr2:uid="{0043E536-1C9D-394E-8ED1-92BEC5123453}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="20820" activeTab="2" xr2:uid="{0043E536-1C9D-394E-8ED1-92BEC5123453}"/>
   </bookViews>
   <sheets>
     <sheet name="RF features" sheetId="2" r:id="rId1"/>

</xml_diff>